<commit_message>
Atualizada á lista de pesquisa
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao/AdvantageOnline_Data.xlsx
+++ b/HubTalentos-Avaliacao/AdvantageOnline_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Git\HubTalentosAvaliacao\HubTalentos-Avaliacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F3B31B-A8BD-4C39-9E52-162834A5BB8D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF361849-53DB-4599-BA14-03EC2071FFCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="2" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
   <si>
     <t>NUMBER TEST</t>
   </si>
@@ -400,6 +400,21 @@
     <t>MICE</t>
   </si>
   <si>
+    <t>HEADPHONES</t>
+  </si>
+  <si>
+    <t>Beats Studio 2 Over-Ear Matte Black Headphones</t>
+  </si>
+  <si>
+    <t>Bose SoundLink Around-ear Wireless Headphones II</t>
+  </si>
+  <si>
+    <t>HP H2310 In-ear Headset</t>
+  </si>
+  <si>
+    <t>Logitech USB Headset H390</t>
+  </si>
+  <si>
     <t>HP USB 3 Button Optical Mouse</t>
   </si>
   <si>
@@ -415,7 +430,7 @@
     <t>HP Z8000 Bluetooth Mouse</t>
   </si>
   <si>
-    <t>Kensington Orbit 72337 Trackball with Scroll Ring</t>
+    <t>Kensington Orbit 72337 Trackball With Scroll Ring</t>
   </si>
   <si>
     <t>Kensington Orbit 72352 Trackball</t>
@@ -425,21 +440,6 @@
   </si>
   <si>
     <t>Microsoft Sculpt Touch Mouse</t>
-  </si>
-  <si>
-    <t>HEADPHONES</t>
-  </si>
-  <si>
-    <t>Beats Studio 2 Over-Ear Matte Black Headphones</t>
-  </si>
-  <si>
-    <t>Bose SoundLink Around-ear Wireless Headphones II</t>
-  </si>
-  <si>
-    <t>HP H2310 In-ear Headset</t>
-  </si>
-  <si>
-    <t>Logitech USB Headset H390</t>
   </si>
 </sst>
 </file>
@@ -500,12 +500,24 @@
       <name val="Aharoni"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -571,7 +583,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -590,6 +602,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1097,13 +1115,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2589F06A-7E62-4BBF-BE1C-16B6DF5BF8F9}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="2" max="2" width="50.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1113,48 +1131,48 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>52</v>
+      <c r="B5" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
-        <v>53</v>
+      <c r="B6" s="9" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
-      <c r="B7" s="5" t="s">
-        <v>54</v>
+      <c r="B7" s="9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
-        <v>55</v>
+      <c r="B8" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1167,7 +1185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADD764A-3ADA-4DFD-BFD9-501D21F8734C}">
   <dimension ref="B1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1178,27 +1196,27 @@
   <sheetData>
     <row r="1" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionada mais uma célula para teste
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao/AdvantageOnline_Data.xlsx
+++ b/HubTalentos-Avaliacao/AdvantageOnline_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Git\HubTalentosAvaliacao\HubTalentos-Avaliacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF361849-53DB-4599-BA14-03EC2071FFCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B149FB-3E46-484F-A15F-761C7EAB079A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>NUMBER TEST</t>
   </si>
@@ -322,9 +322,6 @@
     <t>5200 444</t>
   </si>
   <si>
-    <t>BRUNO383</t>
-  </si>
-  <si>
     <t>2º</t>
   </si>
   <si>
@@ -340,12 +337,6 @@
     <t>marcelamatos@teste.com</t>
   </si>
   <si>
-    <t>Marcela74</t>
-  </si>
-  <si>
-    <t>BrUn-^:1SW</t>
-  </si>
-  <si>
     <t>blumenal@teste.com</t>
   </si>
   <si>
@@ -440,13 +431,55 @@
   </si>
   <si>
     <t>Microsoft Sculpt Touch Mouse</t>
+  </si>
+  <si>
+    <t>machado@teste.com</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Machado</t>
+  </si>
+  <si>
+    <t>11 45 5593 4215</t>
+  </si>
+  <si>
+    <t>Norfolk Islands</t>
+  </si>
+  <si>
+    <t>Kamuli</t>
+  </si>
+  <si>
+    <t>Futton Nine</t>
+  </si>
+  <si>
+    <t>58152 412</t>
+  </si>
+  <si>
+    <t>HP H5H59HX</t>
+  </si>
+  <si>
+    <t>Machado32</t>
+  </si>
+  <si>
+    <t>BRUNO109</t>
+  </si>
+  <si>
+    <t>Marcela103</t>
+  </si>
+  <si>
+    <t>BrUn94</t>
+  </si>
+  <si>
+    <t>Maria14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -499,6 +532,13 @@
       <color theme="1"/>
       <name val="Aharoni"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -520,7 +560,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -578,12 +618,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -608,6 +659,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -925,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA74D7E8-6402-4590-A29D-1B9CE9F8EE2E}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,7 +1051,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
@@ -1025,78 +1086,113 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="G3" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>46</v>
+      <c r="L5" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1104,10 +1200,11 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{506B5F6E-04B9-42F4-B212-FF15B9BD919A}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{F17133B7-2C6B-415C-9D6B-D05BC20E0D31}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{2D786DDF-5728-4B60-AD28-AF599AF8C51C}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{E6835DCD-797E-423A-91F9-44A94D89F401}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1115,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2589F06A-7E62-4BBF-BE1C-16B6DF5BF8F9}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,53 +1223,53 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1183,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADD764A-3ADA-4DFD-BFD9-501D21F8734C}">
-  <dimension ref="B1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,32 +1291,45 @@
     <col min="2" max="2" width="47.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>53</v>
-      </c>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Classe renomeada apenas, sem alteração no código.
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao/AdvantageOnline_Data.xlsx
+++ b/HubTalentos-Avaliacao/AdvantageOnline_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Git\HubTalentosAvaliacao\HubTalentos-Avaliacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B149FB-3E46-484F-A15F-761C7EAB079A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40FA2EF-3E3D-487B-8011-D9FE3F80D76A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="15300" windowHeight="7875" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -463,16 +463,16 @@
     <t>Machado32</t>
   </si>
   <si>
-    <t>BRUNO109</t>
-  </si>
-  <si>
-    <t>Marcela103</t>
-  </si>
-  <si>
-    <t>BrUn94</t>
-  </si>
-  <si>
-    <t>Maria14</t>
+    <t>Marcela104</t>
+  </si>
+  <si>
+    <t>BrUn95</t>
+  </si>
+  <si>
+    <t>Maria15</t>
+  </si>
+  <si>
+    <t>BRUNO114</t>
   </si>
 </sst>
 </file>
@@ -988,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA74D7E8-6402-4590-A29D-1B9CE9F8EE2E}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1051,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
@@ -1089,7 +1089,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>27</v>
@@ -1127,7 +1127,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>28</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>60</v>
@@ -1282,7 +1282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADD764A-3ADA-4DFD-BFD9-501D21F8734C}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Alterações dos nomes de usuário para teste.
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao/AdvantageOnline_Data.xlsx
+++ b/HubTalentos-Avaliacao/AdvantageOnline_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Git\HubTalentosAvaliacao\HubTalentos-Avaliacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40FA2EF-3E3D-487B-8011-D9FE3F80D76A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C8A6E2-5071-4CC5-A81F-D95A49A6F3FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="15300" windowHeight="7875" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -463,16 +463,16 @@
     <t>Machado32</t>
   </si>
   <si>
-    <t>Marcela104</t>
-  </si>
-  <si>
-    <t>BrUn95</t>
-  </si>
-  <si>
-    <t>Maria15</t>
-  </si>
-  <si>
-    <t>BRUNO114</t>
+    <t>BRUNO125</t>
+  </si>
+  <si>
+    <t>Marcela110</t>
+  </si>
+  <si>
+    <t>BrUn97</t>
+  </si>
+  <si>
+    <t>Maria25</t>
   </si>
 </sst>
 </file>
@@ -989,7 +989,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1051,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
@@ -1089,7 +1089,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>27</v>
@@ -1127,7 +1127,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>28</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Sem alterações váldias, apenas formatação de texto.
</commit_message>
<xml_diff>
--- a/HubTalentos-Avaliacao/AdvantageOnline_Data.xlsx
+++ b/HubTalentos-Avaliacao/AdvantageOnline_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Git\HubTalentosAvaliacao\HubTalentos-Avaliacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.junior\Documents\Test\HubTalentosAvaliacao_TDD\HubTalentos-Avaliacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C8A6E2-5071-4CC5-A81F-D95A49A6F3FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707472D5-CC96-41ED-8BF2-C23273888D24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8D0779E8-EFC8-4813-BF37-B00537C68B16}"/>
   </bookViews>
@@ -463,16 +463,16 @@
     <t>Machado32</t>
   </si>
   <si>
-    <t>BRUNO125</t>
-  </si>
-  <si>
     <t>Marcela110</t>
   </si>
   <si>
     <t>BrUn97</t>
   </si>
   <si>
-    <t>Maria25</t>
+    <t>Maria26</t>
+  </si>
+  <si>
+    <t>BRUNO135</t>
   </si>
 </sst>
 </file>
@@ -989,7 +989,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1051,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
@@ -1089,7 +1089,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>27</v>
@@ -1127,7 +1127,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>28</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>60</v>

</xml_diff>